<commit_message>
generate rhodepsin e cathepsinL
</commit_message>
<xml_diff>
--- a/cathepsin/cathepsinL_kinect.xlsx
+++ b/cathepsin/cathepsinL_kinect.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:Z1"/>
+  <dimension ref="A1:Z20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -560,6 +560,1672 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>1814175</v>
+      </c>
+      <c r="B2" t="n">
+        <v>2200847</v>
+      </c>
+      <c r="C2" t="n">
+        <v>467.57</v>
+      </c>
+      <c r="D2" t="n">
+        <v>4.72</v>
+      </c>
+      <c r="E2" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G2" t="n">
+        <v>91.22</v>
+      </c>
+      <c r="H2" t="n">
+        <v>11</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>13.38</v>
+      </c>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="n">
+        <v>5.56</v>
+      </c>
+      <c r="N2" t="n">
+        <v>5.56</v>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="P2" t="n">
+        <v>467.57</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>3</v>
+      </c>
+      <c r="R2" t="n">
+        <v>35</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="T2" t="n">
+        <v>467.2209</v>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>C29H29N3O3</t>
+        </is>
+      </c>
+      <c r="V2" t="n">
+        <v>6</v>
+      </c>
+      <c r="W2" t="n">
+        <v>2</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>CHEMBL4060936</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>N#C/C=C/[C@H](CCc1ccccc1)NC(=O)[C@H](Cc1ccccc1)NC(=O)OCc1ccccc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1825428</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2212186</v>
+      </c>
+      <c r="C3" t="n">
+        <v>450.58</v>
+      </c>
+      <c r="D3" t="n">
+        <v>4.59</v>
+      </c>
+      <c r="E3" t="n">
+        <v>4</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" t="n">
+        <v>84.5</v>
+      </c>
+      <c r="H3" t="n">
+        <v>12</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>13.65</v>
+      </c>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="n">
+        <v>5.26</v>
+      </c>
+      <c r="N3" t="n">
+        <v>5.26</v>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="P3" t="n">
+        <v>450.58</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>2</v>
+      </c>
+      <c r="R3" t="n">
+        <v>33</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="T3" t="n">
+        <v>450.2519</v>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>C27H34N2O4</t>
+        </is>
+      </c>
+      <c r="V3" t="n">
+        <v>6</v>
+      </c>
+      <c r="W3" t="n">
+        <v>2</v>
+      </c>
+      <c r="X3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>CHEMBL4072275</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>CC(=O)/C=C/[C@H](CCc1ccccc1)NC(=O)[C@H](CC(C)C)NC(=O)OCc1ccccc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>1831437</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2218256</v>
+      </c>
+      <c r="C4" t="n">
+        <v>484.6</v>
+      </c>
+      <c r="D4" t="n">
+        <v>4.79</v>
+      </c>
+      <c r="E4" t="n">
+        <v>4</v>
+      </c>
+      <c r="F4" t="n">
+        <v>2</v>
+      </c>
+      <c r="G4" t="n">
+        <v>84.5</v>
+      </c>
+      <c r="H4" t="n">
+        <v>12</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>13.56</v>
+      </c>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="n">
+        <v>5.66</v>
+      </c>
+      <c r="N4" t="n">
+        <v>5.66</v>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="P4" t="n">
+        <v>484.6</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>3</v>
+      </c>
+      <c r="R4" t="n">
+        <v>36</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="T4" t="n">
+        <v>484.2362</v>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>C30H32N2O4</t>
+        </is>
+      </c>
+      <c r="V4" t="n">
+        <v>6</v>
+      </c>
+      <c r="W4" t="n">
+        <v>2</v>
+      </c>
+      <c r="X4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>CHEMBL4078345</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>CC(=O)/C=C/[C@H](CCc1ccccc1)NC(=O)[C@H](Cc1ccccc1)NC(=O)OCc1ccccc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>1843287</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2230217</v>
+      </c>
+      <c r="C5" t="n">
+        <v>478.55</v>
+      </c>
+      <c r="D5" t="n">
+        <v>4.43</v>
+      </c>
+      <c r="E5" t="n">
+        <v>6</v>
+      </c>
+      <c r="F5" t="n">
+        <v>2</v>
+      </c>
+      <c r="G5" t="n">
+        <v>134.36</v>
+      </c>
+      <c r="H5" t="n">
+        <v>12</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>13.02</v>
+      </c>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="n">
+        <v>5.09</v>
+      </c>
+      <c r="N5" t="n">
+        <v>5.09</v>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="P5" t="n">
+        <v>478.55</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>2</v>
+      </c>
+      <c r="R5" t="n">
+        <v>35</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="T5" t="n">
+        <v>478.2216</v>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>C26H30N4O5</t>
+        </is>
+      </c>
+      <c r="V5" t="n">
+        <v>9</v>
+      </c>
+      <c r="W5" t="n">
+        <v>2</v>
+      </c>
+      <c r="X5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>CHEMBL4090306</t>
+        </is>
+      </c>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>CC(C)C[C@H](NC(=O)OCc1ccc([N+](=O)[O-])cc1)C(=O)N[C@H](/C=C/C#N)CCc1ccccc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>1849318</v>
+      </c>
+      <c r="B6" t="n">
+        <v>2236299</v>
+      </c>
+      <c r="C6" t="n">
+        <v>495.58</v>
+      </c>
+      <c r="D6" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E6" t="n">
+        <v>6</v>
+      </c>
+      <c r="F6" t="n">
+        <v>2</v>
+      </c>
+      <c r="G6" t="n">
+        <v>127.64</v>
+      </c>
+      <c r="H6" t="n">
+        <v>13</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>13.21</v>
+      </c>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="N6" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="P6" t="n">
+        <v>495.58</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>2</v>
+      </c>
+      <c r="R6" t="n">
+        <v>36</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="T6" t="n">
+        <v>495.2369</v>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>C27H33N3O6</t>
+        </is>
+      </c>
+      <c r="V6" t="n">
+        <v>9</v>
+      </c>
+      <c r="W6" t="n">
+        <v>2</v>
+      </c>
+      <c r="X6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>CHEMBL4096388</t>
+        </is>
+      </c>
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>CC(=O)/C=C/[C@H](CCc1ccccc1)NC(=O)[C@H](CC(C)C)NC(=O)OCc1ccc([N+](=O)[O-])cc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>1852176</v>
+      </c>
+      <c r="B7" t="n">
+        <v>2239180</v>
+      </c>
+      <c r="C7" t="n">
+        <v>433.55</v>
+      </c>
+      <c r="D7" t="n">
+        <v>4.52</v>
+      </c>
+      <c r="E7" t="n">
+        <v>4</v>
+      </c>
+      <c r="F7" t="n">
+        <v>2</v>
+      </c>
+      <c r="G7" t="n">
+        <v>91.22</v>
+      </c>
+      <c r="H7" t="n">
+        <v>11</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>13.46</v>
+      </c>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="n">
+        <v>5.15</v>
+      </c>
+      <c r="N7" t="n">
+        <v>5.15</v>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="P7" t="n">
+        <v>433.55</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>2</v>
+      </c>
+      <c r="R7" t="n">
+        <v>32</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="T7" t="n">
+        <v>433.2365</v>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>C26H31N3O3</t>
+        </is>
+      </c>
+      <c r="V7" t="n">
+        <v>6</v>
+      </c>
+      <c r="W7" t="n">
+        <v>2</v>
+      </c>
+      <c r="X7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>CHEMBL4099269</t>
+        </is>
+      </c>
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t>CC(C)C[C@H](NC(=O)OCc1ccccc1)C(=O)N[C@H](/C=C/C#N)CCc1ccccc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>1854605</v>
+      </c>
+      <c r="B8" t="n">
+        <v>2241625</v>
+      </c>
+      <c r="C8" t="n">
+        <v>466.58</v>
+      </c>
+      <c r="D8" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="E8" t="n">
+        <v>5</v>
+      </c>
+      <c r="F8" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" t="n">
+        <v>93.73</v>
+      </c>
+      <c r="H8" t="n">
+        <v>12</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>13.58</v>
+      </c>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="n">
+        <v>5.31</v>
+      </c>
+      <c r="N8" t="n">
+        <v>5.31</v>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="P8" t="n">
+        <v>466.58</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>2</v>
+      </c>
+      <c r="R8" t="n">
+        <v>34</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="T8" t="n">
+        <v>466.2468</v>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>C27H34N2O5</t>
+        </is>
+      </c>
+      <c r="V8" t="n">
+        <v>7</v>
+      </c>
+      <c r="W8" t="n">
+        <v>2</v>
+      </c>
+      <c r="X8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y8" t="inlineStr">
+        <is>
+          <t>CHEMBL4101714</t>
+        </is>
+      </c>
+      <c r="Z8" t="inlineStr">
+        <is>
+          <t>COC(=O)/C=C/[C@H](CCc1ccccc1)NC(=O)[C@H](CC(C)C)NC(=O)OCc1ccccc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>1943636</v>
+      </c>
+      <c r="B9" t="n">
+        <v>2343821</v>
+      </c>
+      <c r="C9" t="n">
+        <v>490.55</v>
+      </c>
+      <c r="D9" t="n">
+        <v>4.57</v>
+      </c>
+      <c r="E9" t="n">
+        <v>3</v>
+      </c>
+      <c r="F9" t="n">
+        <v>2</v>
+      </c>
+      <c r="G9" t="n">
+        <v>75.27</v>
+      </c>
+      <c r="H9" t="n">
+        <v>11</v>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>13.52</v>
+      </c>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="n">
+        <v>5.46</v>
+      </c>
+      <c r="N9" t="n">
+        <v>5.46</v>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="P9" t="n">
+        <v>490.55</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>3</v>
+      </c>
+      <c r="R9" t="n">
+        <v>36</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="T9" t="n">
+        <v>490.2068</v>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>C29H28F2N2O3</t>
+        </is>
+      </c>
+      <c r="V9" t="n">
+        <v>5</v>
+      </c>
+      <c r="W9" t="n">
+        <v>2</v>
+      </c>
+      <c r="X9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y9" t="inlineStr">
+        <is>
+          <t>CHEMBL4436812</t>
+        </is>
+      </c>
+      <c r="Z9" t="inlineStr">
+        <is>
+          <t>CC(=O)/C=C/[C@H](CCc1ccccc1)NC(=O)[C@H](Cc1ccccc1)NC(=O)c1cc(F)cc(F)c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>1944738</v>
+      </c>
+      <c r="B10" t="n">
+        <v>2344923</v>
+      </c>
+      <c r="C10" t="n">
+        <v>498.58</v>
+      </c>
+      <c r="D10" t="n">
+        <v>4.02</v>
+      </c>
+      <c r="E10" t="n">
+        <v>5</v>
+      </c>
+      <c r="F10" t="n">
+        <v>2</v>
+      </c>
+      <c r="G10" t="n">
+        <v>93.73</v>
+      </c>
+      <c r="H10" t="n">
+        <v>11</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>13.97</v>
+      </c>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="N10" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="P10" t="n">
+        <v>498.58</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>3</v>
+      </c>
+      <c r="R10" t="n">
+        <v>37</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="T10" t="n">
+        <v>498.2155</v>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>C30H30N2O5</t>
+        </is>
+      </c>
+      <c r="V10" t="n">
+        <v>7</v>
+      </c>
+      <c r="W10" t="n">
+        <v>2</v>
+      </c>
+      <c r="X10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y10" t="inlineStr">
+        <is>
+          <t>CHEMBL4437914</t>
+        </is>
+      </c>
+      <c r="Z10" t="inlineStr">
+        <is>
+          <t>CC(=O)/C=C/[C@H](CCc1ccccc1)NC(=O)[C@H](Cc1ccccc1)NC(=O)c1ccc2c(c1)OCO2</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>1948457</v>
+      </c>
+      <c r="B11" t="n">
+        <v>2348644</v>
+      </c>
+      <c r="C11" t="n">
+        <v>490.55</v>
+      </c>
+      <c r="D11" t="n">
+        <v>4.57</v>
+      </c>
+      <c r="E11" t="n">
+        <v>3</v>
+      </c>
+      <c r="F11" t="n">
+        <v>2</v>
+      </c>
+      <c r="G11" t="n">
+        <v>75.27</v>
+      </c>
+      <c r="H11" t="n">
+        <v>11</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>11.76</v>
+      </c>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="n">
+        <v>5.46</v>
+      </c>
+      <c r="N11" t="n">
+        <v>5.46</v>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="P11" t="n">
+        <v>490.55</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>3</v>
+      </c>
+      <c r="R11" t="n">
+        <v>36</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="T11" t="n">
+        <v>490.2068</v>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>C29H28F2N2O3</t>
+        </is>
+      </c>
+      <c r="V11" t="n">
+        <v>5</v>
+      </c>
+      <c r="W11" t="n">
+        <v>2</v>
+      </c>
+      <c r="X11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y11" t="inlineStr">
+        <is>
+          <t>CHEMBL4441635</t>
+        </is>
+      </c>
+      <c r="Z11" t="inlineStr">
+        <is>
+          <t>CC(=O)/C=C/[C@H](CCc1ccccc1)NC(=O)[C@H](Cc1ccccc1)NC(=O)c1c(F)cccc1F</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>1960215</v>
+      </c>
+      <c r="B12" t="n">
+        <v>2360424</v>
+      </c>
+      <c r="C12" t="n">
+        <v>472.56</v>
+      </c>
+      <c r="D12" t="n">
+        <v>4.43</v>
+      </c>
+      <c r="E12" t="n">
+        <v>3</v>
+      </c>
+      <c r="F12" t="n">
+        <v>2</v>
+      </c>
+      <c r="G12" t="n">
+        <v>75.27</v>
+      </c>
+      <c r="H12" t="n">
+        <v>11</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>13.98</v>
+      </c>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="n">
+        <v>5.31</v>
+      </c>
+      <c r="N12" t="n">
+        <v>5.31</v>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="P12" t="n">
+        <v>472.56</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>3</v>
+      </c>
+      <c r="R12" t="n">
+        <v>35</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="T12" t="n">
+        <v>472.2162</v>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>C29H29FN2O3</t>
+        </is>
+      </c>
+      <c r="V12" t="n">
+        <v>5</v>
+      </c>
+      <c r="W12" t="n">
+        <v>2</v>
+      </c>
+      <c r="X12" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y12" t="inlineStr">
+        <is>
+          <t>CHEMBL4453415</t>
+        </is>
+      </c>
+      <c r="Z12" t="inlineStr">
+        <is>
+          <t>CC(=O)/C=C/[C@H](CCc1ccccc1)NC(=O)[C@H](Cc1ccccc1)NC(=O)c1cccc(F)c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>1963527</v>
+      </c>
+      <c r="B13" t="n">
+        <v>2363736</v>
+      </c>
+      <c r="C13" t="n">
+        <v>476.62</v>
+      </c>
+      <c r="D13" t="n">
+        <v>2.82</v>
+      </c>
+      <c r="E13" t="n">
+        <v>4</v>
+      </c>
+      <c r="F13" t="n">
+        <v>2</v>
+      </c>
+      <c r="G13" t="n">
+        <v>81.75</v>
+      </c>
+      <c r="H13" t="n">
+        <v>10</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="n">
+        <v>7.02</v>
+      </c>
+      <c r="M13" t="n">
+        <v>3.28</v>
+      </c>
+      <c r="N13" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="P13" t="n">
+        <v>476.62</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>2</v>
+      </c>
+      <c r="R13" t="n">
+        <v>35</v>
+      </c>
+      <c r="S13" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="T13" t="n">
+        <v>476.2787</v>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>C28H36N4O3</t>
+        </is>
+      </c>
+      <c r="V13" t="n">
+        <v>7</v>
+      </c>
+      <c r="W13" t="n">
+        <v>2</v>
+      </c>
+      <c r="X13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y13" t="inlineStr">
+        <is>
+          <t>CHEMBL4456727</t>
+        </is>
+      </c>
+      <c r="Z13" t="inlineStr">
+        <is>
+          <t>CC(=O)/C=C/[C@H](CCc1ccccc1)NC(=O)[C@H](Cc1ccccc1)NC(=O)N1CCN(C)CC1</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>1971531</v>
+      </c>
+      <c r="B14" t="n">
+        <v>2371746</v>
+      </c>
+      <c r="C14" t="n">
+        <v>463.58</v>
+      </c>
+      <c r="D14" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="E14" t="n">
+        <v>4</v>
+      </c>
+      <c r="F14" t="n">
+        <v>2</v>
+      </c>
+      <c r="G14" t="n">
+        <v>87.73999999999999</v>
+      </c>
+      <c r="H14" t="n">
+        <v>10</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="n">
+        <v>3.21</v>
+      </c>
+      <c r="N14" t="n">
+        <v>3.21</v>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="P14" t="n">
+        <v>463.58</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>2</v>
+      </c>
+      <c r="R14" t="n">
+        <v>34</v>
+      </c>
+      <c r="S14" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="T14" t="n">
+        <v>463.2471</v>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>C27H33N3O4</t>
+        </is>
+      </c>
+      <c r="V14" t="n">
+        <v>7</v>
+      </c>
+      <c r="W14" t="n">
+        <v>2</v>
+      </c>
+      <c r="X14" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y14" t="inlineStr">
+        <is>
+          <t>CHEMBL4464737</t>
+        </is>
+      </c>
+      <c r="Z14" t="inlineStr">
+        <is>
+          <t>CC(=O)/C=C/[C@H](CCc1ccccc1)NC(=O)[C@H](Cc1ccccc1)NC(=O)N1CCOCC1</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>1981850</v>
+      </c>
+      <c r="B15" t="n">
+        <v>2382072</v>
+      </c>
+      <c r="C15" t="n">
+        <v>472.56</v>
+      </c>
+      <c r="D15" t="n">
+        <v>4.43</v>
+      </c>
+      <c r="E15" t="n">
+        <v>3</v>
+      </c>
+      <c r="F15" t="n">
+        <v>2</v>
+      </c>
+      <c r="G15" t="n">
+        <v>75.27</v>
+      </c>
+      <c r="H15" t="n">
+        <v>11</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J15" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="n">
+        <v>5.31</v>
+      </c>
+      <c r="N15" t="n">
+        <v>5.31</v>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="P15" t="n">
+        <v>472.56</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>3</v>
+      </c>
+      <c r="R15" t="n">
+        <v>35</v>
+      </c>
+      <c r="S15" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="T15" t="n">
+        <v>472.2162</v>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>C29H29FN2O3</t>
+        </is>
+      </c>
+      <c r="V15" t="n">
+        <v>5</v>
+      </c>
+      <c r="W15" t="n">
+        <v>2</v>
+      </c>
+      <c r="X15" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y15" t="inlineStr">
+        <is>
+          <t>CHEMBL4475066</t>
+        </is>
+      </c>
+      <c r="Z15" t="inlineStr">
+        <is>
+          <t>CC(=O)/C=C/[C@H](CCc1ccccc1)NC(=O)[C@H](Cc1ccccc1)NC(=O)c1ccc(F)cc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>1986405</v>
+      </c>
+      <c r="B16" t="n">
+        <v>2386709</v>
+      </c>
+      <c r="C16" t="n">
+        <v>472.56</v>
+      </c>
+      <c r="D16" t="n">
+        <v>4.43</v>
+      </c>
+      <c r="E16" t="n">
+        <v>3</v>
+      </c>
+      <c r="F16" t="n">
+        <v>2</v>
+      </c>
+      <c r="G16" t="n">
+        <v>75.27</v>
+      </c>
+      <c r="H16" t="n">
+        <v>11</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" t="n">
+        <v>13.26</v>
+      </c>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="n">
+        <v>5.31</v>
+      </c>
+      <c r="N16" t="n">
+        <v>5.31</v>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="P16" t="n">
+        <v>472.56</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>3</v>
+      </c>
+      <c r="R16" t="n">
+        <v>35</v>
+      </c>
+      <c r="S16" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="T16" t="n">
+        <v>472.2162</v>
+      </c>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>C29H29FN2O3</t>
+        </is>
+      </c>
+      <c r="V16" t="n">
+        <v>5</v>
+      </c>
+      <c r="W16" t="n">
+        <v>2</v>
+      </c>
+      <c r="X16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y16" t="inlineStr">
+        <is>
+          <t>CHEMBL4515298</t>
+        </is>
+      </c>
+      <c r="Z16" t="inlineStr">
+        <is>
+          <t>CC(=O)/C=C/[C@H](CCc1ccccc1)NC(=O)[C@H](Cc1ccccc1)NC(=O)c1ccccc1F</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>1988054</v>
+      </c>
+      <c r="B17" t="n">
+        <v>2388363</v>
+      </c>
+      <c r="C17" t="n">
+        <v>441.14</v>
+      </c>
+      <c r="D17" t="n">
+        <v>2.65</v>
+      </c>
+      <c r="E17" t="n">
+        <v>4</v>
+      </c>
+      <c r="F17" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" t="n">
+        <v>72.47</v>
+      </c>
+      <c r="H17" t="n">
+        <v>6</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J17" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" t="n">
+        <v>13.85</v>
+      </c>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="n">
+        <v>1.87</v>
+      </c>
+      <c r="N17" t="n">
+        <v>1.87</v>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="P17" t="n">
+        <v>441.14</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>1</v>
+      </c>
+      <c r="R17" t="n">
+        <v>21</v>
+      </c>
+      <c r="S17" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="T17" t="n">
+        <v>438.9089</v>
+      </c>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>C13H15Br2NO4S</t>
+        </is>
+      </c>
+      <c r="V17" t="n">
+        <v>5</v>
+      </c>
+      <c r="W17" t="n">
+        <v>1</v>
+      </c>
+      <c r="X17" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y17" t="inlineStr">
+        <is>
+          <t>CHEMBL4516952</t>
+        </is>
+      </c>
+      <c r="Z17" t="inlineStr">
+        <is>
+          <t>C[C@@H](Oc1ccc(Br)cc1Br)C(=O)NC/C=C/S(C)(=O)=O</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>2033633</v>
+      </c>
+      <c r="B18" t="n">
+        <v>2434885</v>
+      </c>
+      <c r="C18" t="n">
+        <v>427.11</v>
+      </c>
+      <c r="D18" t="n">
+        <v>2.26</v>
+      </c>
+      <c r="E18" t="n">
+        <v>4</v>
+      </c>
+      <c r="F18" t="n">
+        <v>1</v>
+      </c>
+      <c r="G18" t="n">
+        <v>72.47</v>
+      </c>
+      <c r="H18" t="n">
+        <v>6</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J18" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" t="n">
+        <v>13.81</v>
+      </c>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="N18" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="P18" t="n">
+        <v>427.11</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>1</v>
+      </c>
+      <c r="R18" t="n">
+        <v>20</v>
+      </c>
+      <c r="S18" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="T18" t="n">
+        <v>424.8932</v>
+      </c>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>C12H13Br2NO4S</t>
+        </is>
+      </c>
+      <c r="V18" t="n">
+        <v>5</v>
+      </c>
+      <c r="W18" t="n">
+        <v>1</v>
+      </c>
+      <c r="X18" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y18" t="inlineStr">
+        <is>
+          <t>CHEMBL4564457</t>
+        </is>
+      </c>
+      <c r="Z18" t="inlineStr">
+        <is>
+          <t>CS(=O)(=O)/C=C/CNC(=O)COc1ccc(Br)cc1Br</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>2035514</v>
+      </c>
+      <c r="B19" t="n">
+        <v>2436864</v>
+      </c>
+      <c r="C19" t="n">
+        <v>490.55</v>
+      </c>
+      <c r="D19" t="n">
+        <v>4.57</v>
+      </c>
+      <c r="E19" t="n">
+        <v>3</v>
+      </c>
+      <c r="F19" t="n">
+        <v>2</v>
+      </c>
+      <c r="G19" t="n">
+        <v>75.27</v>
+      </c>
+      <c r="H19" t="n">
+        <v>11</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J19" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" t="n">
+        <v>13.06</v>
+      </c>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="n">
+        <v>5.46</v>
+      </c>
+      <c r="N19" t="n">
+        <v>5.46</v>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="P19" t="n">
+        <v>490.55</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>3</v>
+      </c>
+      <c r="R19" t="n">
+        <v>36</v>
+      </c>
+      <c r="S19" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="T19" t="n">
+        <v>490.2068</v>
+      </c>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>C29H28F2N2O3</t>
+        </is>
+      </c>
+      <c r="V19" t="n">
+        <v>5</v>
+      </c>
+      <c r="W19" t="n">
+        <v>2</v>
+      </c>
+      <c r="X19" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y19" t="inlineStr">
+        <is>
+          <t>CHEMBL4566436</t>
+        </is>
+      </c>
+      <c r="Z19" t="inlineStr">
+        <is>
+          <t>CC(=O)/C=C/[C@H](CCc1ccccc1)NC(=O)[C@H](Cc1ccccc1)NC(=O)c1ccc(F)cc1F</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>2052786</v>
+      </c>
+      <c r="B20" t="n">
+        <v>2454722</v>
+      </c>
+      <c r="C20" t="n">
+        <v>489.02</v>
+      </c>
+      <c r="D20" t="n">
+        <v>4.94</v>
+      </c>
+      <c r="E20" t="n">
+        <v>3</v>
+      </c>
+      <c r="F20" t="n">
+        <v>2</v>
+      </c>
+      <c r="G20" t="n">
+        <v>75.27</v>
+      </c>
+      <c r="H20" t="n">
+        <v>11</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="J20" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="n">
+        <v>5.78</v>
+      </c>
+      <c r="N20" t="n">
+        <v>5.78</v>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="P20" t="n">
+        <v>489.02</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>3</v>
+      </c>
+      <c r="R20" t="n">
+        <v>35</v>
+      </c>
+      <c r="S20" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="T20" t="n">
+        <v>488.1867</v>
+      </c>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>C29H29ClN2O3</t>
+        </is>
+      </c>
+      <c r="V20" t="n">
+        <v>5</v>
+      </c>
+      <c r="W20" t="n">
+        <v>2</v>
+      </c>
+      <c r="X20" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y20" t="inlineStr">
+        <is>
+          <t>CHEMBL4584291</t>
+        </is>
+      </c>
+      <c r="Z20" t="inlineStr">
+        <is>
+          <t>CC(=O)/C=C/[C@H](CCc1ccccc1)NC(=O)[C@H](Cc1ccccc1)NC(=O)c1ccc(Cl)cc1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>